<commit_message>
Correction of date format
</commit_message>
<xml_diff>
--- a/src/nomadic/start/data/NOMADS_Library_Worksheet.xlsx
+++ b/src/nomadic/start/data/NOMADS_Library_Worksheet.xlsx
@@ -5,17 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\nomadic\experiment_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\nomadic\src\nomadic\start\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438D6BD7-4F14-47FE-877F-AAE5AECC640C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9097A9-A585-4C14-AAFF-E2264193C1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17532" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="2" r:id="rId1"/>
     <sheet name="nomadic" sheetId="6" state="hidden" r:id="rId2"/>
+    <sheet name="options" sheetId="7" state="hidden" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Post_PCR_DNA_threshold_ngul">options!$B$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t>Date:</t>
   </si>
@@ -673,6 +677,12 @@
   </si>
   <si>
     <t>post_pcr_dna_conc_ngul</t>
+  </si>
+  <si>
+    <t>(save this as the filename)</t>
+  </si>
+  <si>
+    <t>Post PCR DNA threshold (ng / µl)</t>
   </si>
 </sst>
 </file>
@@ -906,33 +916,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -948,6 +931,33 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -991,6 +1001,32 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -1004,23 +1040,6 @@
         </left>
         <right style="thin">
           <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
         </right>
         <top style="thin">
           <color indexed="64"/>
@@ -1049,15 +1068,6 @@
         </bottom>
       </border>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1204,9 +1214,9 @@
   <tableColumns count="5">
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Well" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sample ID" dataDxfId="10"/>
-    <tableColumn id="26" xr3:uid="{CDAB9BF6-0E65-46A9-85EA-6751A98F15D6}" name="Sample Type" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PCR [DNA] (ng / µl)" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Barcode#" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{CDAB9BF6-0E65-46A9-85EA-6751A98F15D6}" name="Sample Type" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PCR [DNA] (ng / µl)" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Barcode#" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1217,13 +1227,13 @@
   <autoFilter ref="A1:D97" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="sample_id"/>
-    <tableColumn id="9" xr3:uid="{98E62512-61AC-41C9-8930-37E9E6964CA3}" name="sample_type" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{98E62512-61AC-41C9-8930-37E9E6964CA3}" name="sample_type" dataDxfId="6">
       <calculatedColumnFormula>IF(LEN(Library!C10)=0,"",Library!C10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="barcode" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="barcode" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(Library!B10),"",CONCATENATE("barcode",Library!E10))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1FDA51E1-A0B8-4EA2-9C5A-4746ACED2260}" name="post_pcr_dna_conc_ngul" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{1FDA51E1-A0B8-4EA2-9C5A-4746ACED2260}" name="post_pcr_dna_conc_ngul" dataDxfId="4">
       <calculatedColumnFormula>IF(LEN(Library!D10)=0,"",Library!D10)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1414,7 +1424,7 @@
   <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1428,56 +1438,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
       <c r="F3" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="11" t="s">
         <v>3</v>
       </c>
@@ -1487,9 +1497,9 @@
         <v>210</v>
       </c>
       <c r="B6" s="26"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="10" t="s">
         <v>209</v>
       </c>
@@ -1499,13 +1509,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="27"/>
-      <c r="C7" s="29" t="str">
+      <c r="C7" s="30" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4), ISBLANK(C5), ISBLANK(C6)),"",CONCATENATE(C2,"_",C3,C5,"_",C4,"_Batch",C6))</f>
         <v/>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="13"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="10" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" s="12"/>
@@ -1534,7 +1546,7 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
@@ -1545,7 +1557,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="31"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1557,7 +1569,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="31"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1568,7 +1580,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="31"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1579,7 +1591,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="31"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1590,7 +1602,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="31"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="3" t="s">
         <v>19</v>
       </c>
@@ -1601,7 +1613,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="31"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="3" t="s">
         <v>21</v>
       </c>
@@ -1612,7 +1624,7 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="32"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="7" t="s">
         <v>23</v>
       </c>
@@ -1623,7 +1635,7 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="30"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1634,7 +1646,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="31"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1645,7 +1657,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="31"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="3" t="s">
         <v>29</v>
       </c>
@@ -1656,7 +1668,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="31"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1667,7 +1679,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="31"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="3" t="s">
         <v>33</v>
       </c>
@@ -1678,7 +1690,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="31"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="3" t="s">
         <v>35</v>
       </c>
@@ -1689,7 +1701,7 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="31"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="3" t="s">
         <v>37</v>
       </c>
@@ -1700,7 +1712,7 @@
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="33"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="9" t="s">
         <v>39</v>
       </c>
@@ -1711,7 +1723,7 @@
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="30"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="5" t="s">
         <v>41</v>
       </c>
@@ -1722,7 +1734,7 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="31"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="3" t="s">
         <v>43</v>
       </c>
@@ -1733,7 +1745,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="31"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="3" t="s">
         <v>45</v>
       </c>
@@ -1744,7 +1756,7 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="31"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="3" t="s">
         <v>47</v>
       </c>
@@ -1755,7 +1767,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="31"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="3" t="s">
         <v>49</v>
       </c>
@@ -1766,7 +1778,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="31"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="3" t="s">
         <v>51</v>
       </c>
@@ -1777,7 +1789,7 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="31"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="3" t="s">
         <v>53</v>
       </c>
@@ -1788,7 +1800,7 @@
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="32"/>
+      <c r="D33" s="24"/>
       <c r="E33" s="7" t="s">
         <v>55</v>
       </c>
@@ -1799,7 +1811,7 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="30"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="5" t="s">
         <v>57</v>
       </c>
@@ -1810,7 +1822,7 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="31"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="3" t="s">
         <v>59</v>
       </c>
@@ -1821,7 +1833,7 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="31"/>
+      <c r="D36" s="23"/>
       <c r="E36" s="3" t="s">
         <v>61</v>
       </c>
@@ -1832,7 +1844,7 @@
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="31"/>
+      <c r="D37" s="23"/>
       <c r="E37" s="3" t="s">
         <v>63</v>
       </c>
@@ -1843,7 +1855,7 @@
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="31"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="3" t="s">
         <v>65</v>
       </c>
@@ -1854,7 +1866,7 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="31"/>
+      <c r="D39" s="23"/>
       <c r="E39" s="3" t="s">
         <v>67</v>
       </c>
@@ -1865,7 +1877,7 @@
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="31"/>
+      <c r="D40" s="23"/>
       <c r="E40" s="3" t="s">
         <v>69</v>
       </c>
@@ -1876,7 +1888,7 @@
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="32"/>
+      <c r="D41" s="24"/>
       <c r="E41" s="7" t="s">
         <v>71</v>
       </c>
@@ -1887,7 +1899,7 @@
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="30"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="5" t="s">
         <v>73</v>
       </c>
@@ -1898,7 +1910,7 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="31"/>
+      <c r="D43" s="23"/>
       <c r="E43" s="3" t="s">
         <v>75</v>
       </c>
@@ -1909,7 +1921,7 @@
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="31"/>
+      <c r="D44" s="23"/>
       <c r="E44" s="3" t="s">
         <v>77</v>
       </c>
@@ -1920,7 +1932,7 @@
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="31"/>
+      <c r="D45" s="23"/>
       <c r="E45" s="3" t="s">
         <v>79</v>
       </c>
@@ -1931,7 +1943,7 @@
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="31"/>
+      <c r="D46" s="23"/>
       <c r="E46" s="3" t="s">
         <v>81</v>
       </c>
@@ -1942,7 +1954,7 @@
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="31"/>
+      <c r="D47" s="23"/>
       <c r="E47" s="3" t="s">
         <v>83</v>
       </c>
@@ -1953,7 +1965,7 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="31"/>
+      <c r="D48" s="23"/>
       <c r="E48" s="3" t="s">
         <v>85</v>
       </c>
@@ -1964,7 +1976,7 @@
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="32"/>
+      <c r="D49" s="24"/>
       <c r="E49" s="7" t="s">
         <v>87</v>
       </c>
@@ -1975,7 +1987,7 @@
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="30"/>
+      <c r="D50" s="22"/>
       <c r="E50" s="5" t="s">
         <v>89</v>
       </c>
@@ -1986,7 +1998,7 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="31"/>
+      <c r="D51" s="23"/>
       <c r="E51" s="3" t="s">
         <v>91</v>
       </c>
@@ -1997,7 +2009,7 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="31"/>
+      <c r="D52" s="23"/>
       <c r="E52" s="3" t="s">
         <v>93</v>
       </c>
@@ -2008,7 +2020,7 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="31"/>
+      <c r="D53" s="23"/>
       <c r="E53" s="3" t="s">
         <v>95</v>
       </c>
@@ -2019,7 +2031,7 @@
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="31"/>
+      <c r="D54" s="23"/>
       <c r="E54" s="3" t="s">
         <v>97</v>
       </c>
@@ -2030,7 +2042,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="31"/>
+      <c r="D55" s="23"/>
       <c r="E55" s="3" t="s">
         <v>99</v>
       </c>
@@ -2041,7 +2053,7 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
-      <c r="D56" s="31"/>
+      <c r="D56" s="23"/>
       <c r="E56" s="3" t="s">
         <v>101</v>
       </c>
@@ -2052,7 +2064,7 @@
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
-      <c r="D57" s="32"/>
+      <c r="D57" s="24"/>
       <c r="E57" s="7" t="s">
         <v>103</v>
       </c>
@@ -2063,7 +2075,7 @@
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
-      <c r="D58" s="30"/>
+      <c r="D58" s="22"/>
       <c r="E58" s="5" t="s">
         <v>105</v>
       </c>
@@ -2074,7 +2086,7 @@
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="31"/>
+      <c r="D59" s="23"/>
       <c r="E59" s="3" t="s">
         <v>107</v>
       </c>
@@ -2085,7 +2097,7 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="31"/>
+      <c r="D60" s="23"/>
       <c r="E60" s="3" t="s">
         <v>109</v>
       </c>
@@ -2096,7 +2108,7 @@
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="31"/>
+      <c r="D61" s="23"/>
       <c r="E61" s="3" t="s">
         <v>111</v>
       </c>
@@ -2107,7 +2119,7 @@
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="31"/>
+      <c r="D62" s="23"/>
       <c r="E62" s="3" t="s">
         <v>113</v>
       </c>
@@ -2118,7 +2130,7 @@
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="31"/>
+      <c r="D63" s="23"/>
       <c r="E63" s="3" t="s">
         <v>115</v>
       </c>
@@ -2129,7 +2141,7 @@
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="31"/>
+      <c r="D64" s="23"/>
       <c r="E64" s="3" t="s">
         <v>117</v>
       </c>
@@ -2140,7 +2152,7 @@
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
-      <c r="D65" s="32"/>
+      <c r="D65" s="24"/>
       <c r="E65" s="7" t="s">
         <v>119</v>
       </c>
@@ -2151,7 +2163,7 @@
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="30"/>
+      <c r="D66" s="22"/>
       <c r="E66" s="5" t="s">
         <v>121</v>
       </c>
@@ -2162,7 +2174,7 @@
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
-      <c r="D67" s="31"/>
+      <c r="D67" s="23"/>
       <c r="E67" s="3" t="s">
         <v>123</v>
       </c>
@@ -2173,7 +2185,7 @@
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
-      <c r="D68" s="31"/>
+      <c r="D68" s="23"/>
       <c r="E68" s="3" t="s">
         <v>125</v>
       </c>
@@ -2184,7 +2196,7 @@
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
-      <c r="D69" s="31"/>
+      <c r="D69" s="23"/>
       <c r="E69" s="3" t="s">
         <v>127</v>
       </c>
@@ -2195,7 +2207,7 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
-      <c r="D70" s="31"/>
+      <c r="D70" s="23"/>
       <c r="E70" s="3" t="s">
         <v>129</v>
       </c>
@@ -2206,7 +2218,7 @@
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
-      <c r="D71" s="31"/>
+      <c r="D71" s="23"/>
       <c r="E71" s="3" t="s">
         <v>131</v>
       </c>
@@ -2217,7 +2229,7 @@
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
-      <c r="D72" s="31"/>
+      <c r="D72" s="23"/>
       <c r="E72" s="3" t="s">
         <v>133</v>
       </c>
@@ -2228,7 +2240,7 @@
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
-      <c r="D73" s="32"/>
+      <c r="D73" s="24"/>
       <c r="E73" s="7" t="s">
         <v>135</v>
       </c>
@@ -2239,7 +2251,7 @@
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="30"/>
+      <c r="D74" s="22"/>
       <c r="E74" s="5" t="s">
         <v>137</v>
       </c>
@@ -2250,7 +2262,7 @@
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="31"/>
+      <c r="D75" s="23"/>
       <c r="E75" s="3" t="s">
         <v>139</v>
       </c>
@@ -2261,7 +2273,7 @@
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="31"/>
+      <c r="D76" s="23"/>
       <c r="E76" s="3" t="s">
         <v>141</v>
       </c>
@@ -2272,7 +2284,7 @@
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="31"/>
+      <c r="D77" s="23"/>
       <c r="E77" s="3" t="s">
         <v>143</v>
       </c>
@@ -2283,7 +2295,7 @@
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
-      <c r="D78" s="31"/>
+      <c r="D78" s="23"/>
       <c r="E78" s="3" t="s">
         <v>145</v>
       </c>
@@ -2294,7 +2306,7 @@
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
-      <c r="D79" s="31"/>
+      <c r="D79" s="23"/>
       <c r="E79" s="3" t="s">
         <v>147</v>
       </c>
@@ -2305,7 +2317,7 @@
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
-      <c r="D80" s="31"/>
+      <c r="D80" s="23"/>
       <c r="E80" s="3" t="s">
         <v>149</v>
       </c>
@@ -2316,7 +2328,7 @@
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
-      <c r="D81" s="32"/>
+      <c r="D81" s="24"/>
       <c r="E81" s="7" t="s">
         <v>151</v>
       </c>
@@ -2327,7 +2339,7 @@
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
-      <c r="D82" s="30"/>
+      <c r="D82" s="22"/>
       <c r="E82" s="5" t="s">
         <v>153</v>
       </c>
@@ -2338,7 +2350,7 @@
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
-      <c r="D83" s="31"/>
+      <c r="D83" s="23"/>
       <c r="E83" s="3" t="s">
         <v>155</v>
       </c>
@@ -2349,7 +2361,7 @@
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
-      <c r="D84" s="31"/>
+      <c r="D84" s="23"/>
       <c r="E84" s="3" t="s">
         <v>157</v>
       </c>
@@ -2360,7 +2372,7 @@
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
-      <c r="D85" s="31"/>
+      <c r="D85" s="23"/>
       <c r="E85" s="3" t="s">
         <v>159</v>
       </c>
@@ -2371,7 +2383,7 @@
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
-      <c r="D86" s="31"/>
+      <c r="D86" s="23"/>
       <c r="E86" s="3" t="s">
         <v>161</v>
       </c>
@@ -2382,7 +2394,7 @@
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="31"/>
+      <c r="D87" s="23"/>
       <c r="E87" s="3" t="s">
         <v>163</v>
       </c>
@@ -2393,7 +2405,7 @@
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
-      <c r="D88" s="31"/>
+      <c r="D88" s="23"/>
       <c r="E88" s="3" t="s">
         <v>165</v>
       </c>
@@ -2404,7 +2416,7 @@
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
-      <c r="D89" s="32"/>
+      <c r="D89" s="24"/>
       <c r="E89" s="7" t="s">
         <v>167</v>
       </c>
@@ -2415,7 +2427,7 @@
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
-      <c r="D90" s="30"/>
+      <c r="D90" s="22"/>
       <c r="E90" s="5" t="s">
         <v>169</v>
       </c>
@@ -2426,7 +2438,7 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="31"/>
+      <c r="D91" s="23"/>
       <c r="E91" s="3" t="s">
         <v>171</v>
       </c>
@@ -2437,7 +2449,7 @@
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="D92" s="31"/>
+      <c r="D92" s="23"/>
       <c r="E92" s="3" t="s">
         <v>173</v>
       </c>
@@ -2448,7 +2460,7 @@
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
-      <c r="D93" s="31"/>
+      <c r="D93" s="23"/>
       <c r="E93" s="3" t="s">
         <v>175</v>
       </c>
@@ -2459,7 +2471,7 @@
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
-      <c r="D94" s="31"/>
+      <c r="D94" s="23"/>
       <c r="E94" s="3" t="s">
         <v>177</v>
       </c>
@@ -2470,7 +2482,7 @@
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="31"/>
+      <c r="D95" s="23"/>
       <c r="E95" s="3" t="s">
         <v>179</v>
       </c>
@@ -2481,7 +2493,7 @@
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="31"/>
+      <c r="D96" s="23"/>
       <c r="E96" s="3" t="s">
         <v>181</v>
       </c>
@@ -2492,7 +2504,7 @@
       </c>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
-      <c r="D97" s="32"/>
+      <c r="D97" s="24"/>
       <c r="E97" s="7" t="s">
         <v>183</v>
       </c>
@@ -2503,7 +2515,7 @@
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
-      <c r="D98" s="30"/>
+      <c r="D98" s="22"/>
       <c r="E98" s="5" t="s">
         <v>185</v>
       </c>
@@ -2514,7 +2526,7 @@
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
-      <c r="D99" s="31"/>
+      <c r="D99" s="23"/>
       <c r="E99" s="3" t="s">
         <v>187</v>
       </c>
@@ -2525,7 +2537,7 @@
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="31"/>
+      <c r="D100" s="23"/>
       <c r="E100" s="3" t="s">
         <v>189</v>
       </c>
@@ -2536,7 +2548,7 @@
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
-      <c r="D101" s="31"/>
+      <c r="D101" s="23"/>
       <c r="E101" s="3" t="s">
         <v>191</v>
       </c>
@@ -2547,7 +2559,7 @@
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
-      <c r="D102" s="31"/>
+      <c r="D102" s="23"/>
       <c r="E102" s="3" t="s">
         <v>193</v>
       </c>
@@ -2558,7 +2570,7 @@
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
-      <c r="D103" s="31"/>
+      <c r="D103" s="23"/>
       <c r="E103" s="3" t="s">
         <v>195</v>
       </c>
@@ -2569,7 +2581,7 @@
       </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="31"/>
+      <c r="D104" s="23"/>
       <c r="E104" s="3" t="s">
         <v>197</v>
       </c>
@@ -2580,7 +2592,7 @@
       </c>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
-      <c r="D105" s="32"/>
+      <c r="D105" s="24"/>
       <c r="E105" s="7" t="s">
         <v>199</v>
       </c>
@@ -2666,13 +2678,8 @@
       <c r="F115" s="13"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C3:E3"/>
@@ -2680,6 +2687,12 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B10:E105">
@@ -2695,10 +2708,10 @@
   <conditionalFormatting sqref="D10:D105">
     <cfRule type="cellIs" dxfId="1" priority="6" operator="between">
       <formula>0</formula>
-      <formula>15</formula>
+      <formula>Post_PCR_DNA_threshold_ngul</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThanOrEqual">
-      <formula>15</formula>
+      <formula>Post_PCR_DNA_threshold_ngul</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="9">
@@ -2721,9 +2734,8 @@
       <formula1>0.0000000000000001</formula1>
       <formula2>9999999999</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a Date" error="Please check your entry and ensure it is a date in the format YYY-MM-DD e.g. 2024-10-28" sqref="C2:E2" xr:uid="{6948A87B-14F5-4864-A3CB-3A5971E46210}">
-      <formula1>43831</formula1>
-      <formula2>TODAY()</formula2>
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a Date" error="Please check your entry and ensure it is a date in the format YYYY-MM-DD e.g. 2024-10-28" sqref="C2:E2" xr:uid="{6948A87B-14F5-4864-A3CB-3A5971E46210}">
+      <formula1>10</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Number of initials" error="Please just enter the first and last name initials e.g. John Smith = JS" sqref="C3:E3" xr:uid="{6E22CD84-505D-440D-BC75-9483B6185E39}">
       <formula1>2</formula1>
@@ -4505,4 +4517,33 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5817B840-46A1-4DBD-A947-D1215FFA570B}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added barcodes back in by default, but also highlight any duplicate barcodes
</commit_message>
<xml_diff>
--- a/src/nomadic/start/data/NOMADS_Library_Worksheet.xlsx
+++ b/src/nomadic/start/data/NOMADS_Library_Worksheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\nomadic\src\nomadic\start\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D0D839-F76C-4A4E-8712-FCF79450F02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F101C0C-1770-4895-A4F6-CEE10C0C6F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46284" windowHeight="23244" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="27276" windowHeight="15456" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="2" r:id="rId1"/>
     <sheet name="Gel" sheetId="8" r:id="rId2"/>
-    <sheet name="nomadic" sheetId="6" r:id="rId3"/>
+    <sheet name="nomadic" sheetId="6" state="hidden" r:id="rId3"/>
     <sheet name="options" sheetId="7" state="hidden" r:id="rId4"/>
     <sheet name="Instructions" sheetId="9" r:id="rId5"/>
   </sheets>
@@ -639,7 +639,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -712,38 +712,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -766,8 +735,35 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -779,7 +775,213 @@
     <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -821,46 +1023,6 @@
         </bottom>
       </border>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1215,14 +1377,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_SeqLib" displayName="tbl_SeqLib" ref="A9:E105" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_SeqLib" displayName="tbl_SeqLib" ref="A9:E105" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A9:E105" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Well" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sample ID" dataDxfId="10"/>
-    <tableColumn id="26" xr3:uid="{CDAB9BF6-0E65-46A9-85EA-6751A98F15D6}" name="Sample Type" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PCR [DNA] (ng / µl)" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Barcode" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Well" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sample ID" dataDxfId="32"/>
+    <tableColumn id="26" xr3:uid="{CDAB9BF6-0E65-46A9-85EA-6751A98F15D6}" name="Sample Type" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PCR [DNA] (ng / µl)" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Barcode" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1233,13 +1395,13 @@
   <autoFilter ref="A1:D97" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="sample_id"/>
-    <tableColumn id="9" xr3:uid="{98E62512-61AC-41C9-8930-37E9E6964CA3}" name="sample_type" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{98E62512-61AC-41C9-8930-37E9E6964CA3}" name="sample_type" dataDxfId="28">
       <calculatedColumnFormula>IF(LEN(Library!C10)=0,"",Library!C10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="barcode" dataDxfId="7">
-      <calculatedColumnFormula>IF(ISBLANK(Library!B10),"",CONCATENATE("barcode",Library!E10))</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="barcode" dataDxfId="26">
+      <calculatedColumnFormula>IF(OR(ISBLANK(Library!E10),ISBLANK(Library!B10)),"",CONCATENATE("barcode",TEXT(Library!E10,"00")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1FDA51E1-A0B8-4EA2-9C5A-4746ACED2260}" name="post_pcr_dna_conc_ngul" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{1FDA51E1-A0B8-4EA2-9C5A-4746ACED2260}" name="post_pcr_dna_conc_ngul" dataDxfId="27">
       <calculatedColumnFormula>IF(LEN(Library!D10)=0,"",Library!D10)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1427,15 +1589,15 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.296875" customWidth="1"/>
+    <col min="1" max="1" width="9.8984375" customWidth="1"/>
     <col min="2" max="2" width="30.3984375" customWidth="1"/>
     <col min="3" max="3" width="24.3984375" customWidth="1"/>
     <col min="4" max="4" width="28.5" customWidth="1"/>
@@ -1443,92 +1605,92 @@
     <col min="6" max="6" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
       <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
       <c r="F3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="29" t="str">
+      <c r="B7" s="33"/>
+      <c r="C7" s="36" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4), ISBLANK(C5), ISBLANK(C6)),"",CONCATENATE(C2,"_",C3,TEXT(C5,"000"),"_",C4,"_Batch",C6))</f>
         <v/>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1544,793 +1706,1311 @@
       <c r="E9" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="18"/>
-      <c r="E10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="29">
+        <v>1</v>
+      </c>
+      <c r="F10" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="19"/>
-      <c r="E11" s="39"/>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="30">
+        <v>2</v>
+      </c>
+      <c r="F11" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="39"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="30">
+        <v>3</v>
+      </c>
+      <c r="F12" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="19"/>
-      <c r="E13" s="39"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="30">
+        <v>4</v>
+      </c>
+      <c r="F13" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="19"/>
-      <c r="E14" s="39"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="30">
+        <v>5</v>
+      </c>
+      <c r="F14" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="19"/>
-      <c r="E15" s="39"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="30">
+        <v>6</v>
+      </c>
+      <c r="F15" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="39"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="30">
+        <v>7</v>
+      </c>
+      <c r="F16" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="20"/>
-      <c r="E17" s="40"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="31">
+        <v>8</v>
+      </c>
+      <c r="F17" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="38"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="29">
+        <v>9</v>
+      </c>
+      <c r="F18" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="39"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="30">
+        <v>10</v>
+      </c>
+      <c r="F19" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="39"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="30">
+        <v>11</v>
+      </c>
+      <c r="F20" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="19"/>
-      <c r="E21" s="39"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="30">
+        <v>12</v>
+      </c>
+      <c r="F21" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="19"/>
-      <c r="E22" s="39"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="30">
+        <v>13</v>
+      </c>
+      <c r="F22" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="19"/>
-      <c r="E23" s="39"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="30">
+        <v>14</v>
+      </c>
+      <c r="F23" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="19"/>
-      <c r="E24" s="39"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="30">
+        <v>15</v>
+      </c>
+      <c r="F24" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="21"/>
-      <c r="E25" s="41"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="31">
+        <v>16</v>
+      </c>
+      <c r="F25" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="38"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="29">
+        <v>17</v>
+      </c>
+      <c r="F26" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="19"/>
-      <c r="E27" s="39"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="30">
+        <v>18</v>
+      </c>
+      <c r="F27" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="19"/>
-      <c r="E28" s="39"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="30">
+        <v>19</v>
+      </c>
+      <c r="F28" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="19"/>
-      <c r="E29" s="39"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="30">
+        <v>20</v>
+      </c>
+      <c r="F29" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="19"/>
-      <c r="E30" s="39"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="30">
+        <v>21</v>
+      </c>
+      <c r="F30" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="19"/>
-      <c r="E31" s="39"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="30">
+        <v>22</v>
+      </c>
+      <c r="F31" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="19"/>
-      <c r="E32" s="39"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E32" s="30">
+        <v>23</v>
+      </c>
+      <c r="F32" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="20"/>
-      <c r="E33" s="40"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="31">
+        <v>24</v>
+      </c>
+      <c r="F33" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="18"/>
-      <c r="E34" s="38"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E34" s="29">
+        <v>25</v>
+      </c>
+      <c r="F34" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="19"/>
-      <c r="E35" s="39"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="30">
+        <v>26</v>
+      </c>
+      <c r="F35" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="19"/>
-      <c r="E36" s="39"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="30">
+        <v>27</v>
+      </c>
+      <c r="F36" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="19"/>
-      <c r="E37" s="39"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="30">
+        <v>28</v>
+      </c>
+      <c r="F37" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="19"/>
-      <c r="E38" s="39"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="30">
+        <v>29</v>
+      </c>
+      <c r="F38" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>35</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="19"/>
-      <c r="E39" s="39"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="30">
+        <v>30</v>
+      </c>
+      <c r="F39" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="19"/>
-      <c r="E40" s="39"/>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E40" s="30">
+        <v>31</v>
+      </c>
+      <c r="F40" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="20"/>
-      <c r="E41" s="40"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E41" s="31">
+        <v>32</v>
+      </c>
+      <c r="F41" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="18"/>
-      <c r="E42" s="38"/>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E42" s="29">
+        <v>33</v>
+      </c>
+      <c r="F42" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="19"/>
-      <c r="E43" s="39"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E43" s="30">
+        <v>34</v>
+      </c>
+      <c r="F43" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="19"/>
-      <c r="E44" s="39"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E44" s="30">
+        <v>35</v>
+      </c>
+      <c r="F44" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="19"/>
-      <c r="E45" s="39"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E45" s="30">
+        <v>36</v>
+      </c>
+      <c r="F45" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="19"/>
-      <c r="E46" s="39"/>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E46" s="30">
+        <v>37</v>
+      </c>
+      <c r="F46" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="19"/>
-      <c r="E47" s="39"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="30">
+        <v>38</v>
+      </c>
+      <c r="F47" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="19"/>
-      <c r="E48" s="39"/>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E48" s="30">
+        <v>39</v>
+      </c>
+      <c r="F48" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="20"/>
-      <c r="E49" s="40"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E49" s="31">
+        <v>40</v>
+      </c>
+      <c r="F49" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="18"/>
-      <c r="E50" s="38"/>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E50" s="29">
+        <v>41</v>
+      </c>
+      <c r="F50" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="19"/>
-      <c r="E51" s="39"/>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E51" s="30">
+        <v>42</v>
+      </c>
+      <c r="F51" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="19"/>
-      <c r="E52" s="39"/>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E52" s="30">
+        <v>43</v>
+      </c>
+      <c r="F52" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="19"/>
-      <c r="E53" s="39"/>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E53" s="30">
+        <v>44</v>
+      </c>
+      <c r="F53" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="19"/>
-      <c r="E54" s="39"/>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E54" s="30">
+        <v>45</v>
+      </c>
+      <c r="F54" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="19"/>
-      <c r="E55" s="39"/>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E55" s="30">
+        <v>46</v>
+      </c>
+      <c r="F55" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="19"/>
-      <c r="E56" s="39"/>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E56" s="30">
+        <v>47</v>
+      </c>
+      <c r="F56" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="20"/>
-      <c r="E57" s="40"/>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E57" s="31">
+        <v>48</v>
+      </c>
+      <c r="F57" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="18"/>
-      <c r="E58" s="38"/>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E58" s="29">
+        <v>49</v>
+      </c>
+      <c r="F58" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="19"/>
-      <c r="E59" s="39"/>
-    </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E59" s="30">
+        <v>50</v>
+      </c>
+      <c r="F59" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="19"/>
-      <c r="E60" s="39"/>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E60" s="30">
+        <v>51</v>
+      </c>
+      <c r="F60" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="19"/>
-      <c r="E61" s="39"/>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E61" s="30">
+        <v>52</v>
+      </c>
+      <c r="F61" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="19"/>
-      <c r="E62" s="39"/>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E62" s="30">
+        <v>53</v>
+      </c>
+      <c r="F62" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="s">
         <v>59</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="19"/>
-      <c r="E63" s="39"/>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E63" s="30">
+        <v>54</v>
+      </c>
+      <c r="F63" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="19"/>
-      <c r="E64" s="39"/>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E64" s="30">
+        <v>55</v>
+      </c>
+      <c r="F64" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="16" t="s">
         <v>61</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="20"/>
-      <c r="E65" s="40"/>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E65" s="31">
+        <v>56</v>
+      </c>
+      <c r="F65" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="18"/>
-      <c r="E66" s="38"/>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E66" s="29">
+        <v>57</v>
+      </c>
+      <c r="F66" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="19"/>
-      <c r="E67" s="39"/>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E67" s="30">
+        <v>58</v>
+      </c>
+      <c r="F67" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>64</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="19"/>
-      <c r="E68" s="39"/>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E68" s="30">
+        <v>59</v>
+      </c>
+      <c r="F68" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>65</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="19"/>
-      <c r="E69" s="39"/>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E69" s="30">
+        <v>60</v>
+      </c>
+      <c r="F69" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="19"/>
-      <c r="E70" s="39"/>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E70" s="30">
+        <v>61</v>
+      </c>
+      <c r="F70" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
         <v>67</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="19"/>
-      <c r="E71" s="39"/>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E71" s="30">
+        <v>62</v>
+      </c>
+      <c r="F71" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="19"/>
-      <c r="E72" s="39"/>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E72" s="30">
+        <v>63</v>
+      </c>
+      <c r="F72" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="16" t="s">
         <v>69</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="20"/>
-      <c r="E73" s="40"/>
-    </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E73" s="31">
+        <v>64</v>
+      </c>
+      <c r="F73" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="14" t="s">
         <v>70</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="18"/>
-      <c r="E74" s="38"/>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E74" s="29">
+        <v>65</v>
+      </c>
+      <c r="F74" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="19"/>
-      <c r="E75" s="39"/>
-    </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E75" s="30">
+        <v>66</v>
+      </c>
+      <c r="F75" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="19"/>
-      <c r="E76" s="39"/>
-    </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E76" s="30">
+        <v>67</v>
+      </c>
+      <c r="F76" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>73</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="19"/>
-      <c r="E77" s="39"/>
-    </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E77" s="30">
+        <v>68</v>
+      </c>
+      <c r="F77" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="19"/>
-      <c r="E78" s="39"/>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E78" s="30">
+        <v>69</v>
+      </c>
+      <c r="F78" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="19"/>
-      <c r="E79" s="39"/>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E79" s="30">
+        <v>70</v>
+      </c>
+      <c r="F79" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>76</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="19"/>
-      <c r="E80" s="39"/>
-    </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E80" s="30">
+        <v>71</v>
+      </c>
+      <c r="F80" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="16" t="s">
         <v>77</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="20"/>
-      <c r="E81" s="40"/>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E81" s="31">
+        <v>72</v>
+      </c>
+      <c r="F81" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="18"/>
-      <c r="E82" s="38"/>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E82" s="29">
+        <v>73</v>
+      </c>
+      <c r="F82" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="15" t="s">
         <v>79</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="19"/>
-      <c r="E83" s="39"/>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E83" s="30">
+        <v>74</v>
+      </c>
+      <c r="F83" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="s">
         <v>80</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="19"/>
-      <c r="E84" s="39"/>
-    </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E84" s="30">
+        <v>75</v>
+      </c>
+      <c r="F84" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15" t="s">
         <v>81</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="19"/>
-      <c r="E85" s="39"/>
-    </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E85" s="30">
+        <v>76</v>
+      </c>
+      <c r="F85" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="19"/>
-      <c r="E86" s="39"/>
-    </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E86" s="30">
+        <v>77</v>
+      </c>
+      <c r="F86" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="15" t="s">
         <v>83</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="19"/>
-      <c r="E87" s="39"/>
-    </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E87" s="30">
+        <v>78</v>
+      </c>
+      <c r="F87" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="15" t="s">
         <v>84</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="19"/>
-      <c r="E88" s="39"/>
-    </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E88" s="30">
+        <v>79</v>
+      </c>
+      <c r="F88" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="16" t="s">
         <v>85</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="20"/>
-      <c r="E89" s="40"/>
-    </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E89" s="31">
+        <v>80</v>
+      </c>
+      <c r="F89" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="14" t="s">
         <v>86</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="18"/>
-      <c r="E90" s="38"/>
-    </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E90" s="29">
+        <v>81</v>
+      </c>
+      <c r="F90" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
         <v>87</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="19"/>
-      <c r="E91" s="39"/>
-    </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E91" s="30">
+        <v>82</v>
+      </c>
+      <c r="F91" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="15" t="s">
         <v>88</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="19"/>
-      <c r="E92" s="39"/>
-    </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E92" s="30">
+        <v>83</v>
+      </c>
+      <c r="F92" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>89</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="19"/>
-      <c r="E93" s="39"/>
-    </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E93" s="30">
+        <v>84</v>
+      </c>
+      <c r="F93" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="15" t="s">
         <v>90</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="19"/>
-      <c r="E94" s="39"/>
-    </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E94" s="30">
+        <v>85</v>
+      </c>
+      <c r="F94" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
         <v>91</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="19"/>
-      <c r="E95" s="39"/>
-    </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E95" s="30">
+        <v>86</v>
+      </c>
+      <c r="F95" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
         <v>92</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="19"/>
-      <c r="E96" s="39"/>
+      <c r="E96" s="30">
+        <v>87</v>
+      </c>
+      <c r="F96" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="16" t="s">
@@ -2339,7 +3019,13 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="20"/>
-      <c r="E97" s="40"/>
+      <c r="E97" s="31">
+        <v>88</v>
+      </c>
+      <c r="F97" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
@@ -2348,7 +3034,13 @@
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="18"/>
-      <c r="E98" s="38"/>
+      <c r="E98" s="29">
+        <v>89</v>
+      </c>
+      <c r="F98" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="15" t="s">
@@ -2357,7 +3049,13 @@
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="19"/>
-      <c r="E99" s="39"/>
+      <c r="E99" s="30">
+        <v>90</v>
+      </c>
+      <c r="F99" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="15" t="s">
@@ -2366,7 +3064,13 @@
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="19"/>
-      <c r="E100" s="39"/>
+      <c r="E100" s="30">
+        <v>91</v>
+      </c>
+      <c r="F100" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="15" t="s">
@@ -2375,7 +3079,13 @@
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="19"/>
-      <c r="E101" s="39"/>
+      <c r="E101" s="30">
+        <v>92</v>
+      </c>
+      <c r="F101" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="15" t="s">
@@ -2384,7 +3094,13 @@
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="19"/>
-      <c r="E102" s="39"/>
+      <c r="E102" s="30">
+        <v>93</v>
+      </c>
+      <c r="F102" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="15" t="s">
@@ -2393,7 +3109,13 @@
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="19"/>
-      <c r="E103" s="39"/>
+      <c r="E103" s="30">
+        <v>94</v>
+      </c>
+      <c r="F103" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
@@ -2402,7 +3124,13 @@
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="19"/>
-      <c r="E104" s="39"/>
+      <c r="E104" s="30">
+        <v>95</v>
+      </c>
+      <c r="F104" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="105" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="16" t="s">
@@ -2411,7 +3139,13 @@
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="20"/>
-      <c r="E105" s="40"/>
+      <c r="E105" s="31">
+        <v>96</v>
+      </c>
+      <c r="F105" t="str">
+        <f>IF(COUNTIF(tbl_SeqLib[Barcode],tbl_SeqLib[[#This Row],[Barcode]])&gt;1,"DUPLICATE","")</f>
+        <v/>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="9"/>
@@ -2495,12 +3229,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C3:E3"/>
@@ -2508,25 +3236,39 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B10:E105">
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
       <formula>COUNTIF(B10,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C6">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>COUNTIF(C2,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D105">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="between">
       <formula>0</formula>
       <formula>Post_PCR_DNA_threshold_ngul</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThanOrEqual">
       <formula>Post_PCR_DNA_threshold_ngul</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E105">
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:F105">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Duplicate">
+      <formula>NOT(ISERROR(SEARCH("Duplicate",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="8">
@@ -2594,7 +3336,7 @@
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2628,7 +3370,7 @@
         <v/>
       </c>
       <c r="C2" t="str">
-        <f>IF(ISBLANK(Library!B10),"",CONCATENATE("barcode",Library!E10))</f>
+        <f>IF(OR(ISBLANK(Library!E10),ISBLANK(Library!B10)),"",CONCATENATE("barcode",TEXT(Library!E10,"00")))</f>
         <v/>
       </c>
       <c r="D2" t="str">
@@ -2646,7 +3388,7 @@
         <v/>
       </c>
       <c r="C3" t="str">
-        <f>IF(ISBLANK(Library!B11),"",CONCATENATE("barcode",Library!E11))</f>
+        <f>IF(OR(ISBLANK(Library!E11),ISBLANK(Library!B11)),"",CONCATENATE("barcode",TEXT(Library!E11,"00")))</f>
         <v/>
       </c>
       <c r="D3" t="str">
@@ -2664,7 +3406,7 @@
         <v/>
       </c>
       <c r="C4" t="str">
-        <f>IF(ISBLANK(Library!B12),"",CONCATENATE("barcode",Library!E12))</f>
+        <f>IF(OR(ISBLANK(Library!E12),ISBLANK(Library!B12)),"",CONCATENATE("barcode",TEXT(Library!E12,"00")))</f>
         <v/>
       </c>
       <c r="D4" t="str">
@@ -2682,7 +3424,7 @@
         <v/>
       </c>
       <c r="C5" t="str">
-        <f>IF(ISBLANK(Library!B13),"",CONCATENATE("barcode",Library!E13))</f>
+        <f>IF(OR(ISBLANK(Library!E13),ISBLANK(Library!B13)),"",CONCATENATE("barcode",TEXT(Library!E13,"00")))</f>
         <v/>
       </c>
       <c r="D5" t="str">
@@ -2700,7 +3442,7 @@
         <v/>
       </c>
       <c r="C6" t="str">
-        <f>IF(ISBLANK(Library!B14),"",CONCATENATE("barcode",Library!E14))</f>
+        <f>IF(OR(ISBLANK(Library!E14),ISBLANK(Library!B14)),"",CONCATENATE("barcode",TEXT(Library!E14,"00")))</f>
         <v/>
       </c>
       <c r="D6" t="str">
@@ -2718,7 +3460,7 @@
         <v/>
       </c>
       <c r="C7" t="str">
-        <f>IF(ISBLANK(Library!B15),"",CONCATENATE("barcode",Library!E15))</f>
+        <f>IF(OR(ISBLANK(Library!E15),ISBLANK(Library!B15)),"",CONCATENATE("barcode",TEXT(Library!E15,"00")))</f>
         <v/>
       </c>
       <c r="D7" t="str">
@@ -2736,7 +3478,7 @@
         <v/>
       </c>
       <c r="C8" t="str">
-        <f>IF(ISBLANK(Library!B16),"",CONCATENATE("barcode",Library!E16))</f>
+        <f>IF(OR(ISBLANK(Library!E16),ISBLANK(Library!B16)),"",CONCATENATE("barcode",TEXT(Library!E16,"00")))</f>
         <v/>
       </c>
       <c r="D8" t="str">
@@ -2754,7 +3496,7 @@
         <v/>
       </c>
       <c r="C9" t="str">
-        <f>IF(ISBLANK(Library!B17),"",CONCATENATE("barcode",Library!E17))</f>
+        <f>IF(OR(ISBLANK(Library!E17),ISBLANK(Library!B17)),"",CONCATENATE("barcode",TEXT(Library!E17,"00")))</f>
         <v/>
       </c>
       <c r="D9" t="str">
@@ -2772,7 +3514,7 @@
         <v/>
       </c>
       <c r="C10" t="str">
-        <f>IF(ISBLANK(Library!B18),"",CONCATENATE("barcode",Library!E18))</f>
+        <f>IF(OR(ISBLANK(Library!E18),ISBLANK(Library!B18)),"",CONCATENATE("barcode",TEXT(Library!E18,"00")))</f>
         <v/>
       </c>
       <c r="D10" t="str">
@@ -2790,7 +3532,7 @@
         <v/>
       </c>
       <c r="C11" t="str">
-        <f>IF(ISBLANK(Library!B19),"",CONCATENATE("barcode",Library!E19))</f>
+        <f>IF(OR(ISBLANK(Library!E19),ISBLANK(Library!B19)),"",CONCATENATE("barcode",TEXT(Library!E19,"00")))</f>
         <v/>
       </c>
       <c r="D11" t="str">
@@ -2808,7 +3550,7 @@
         <v/>
       </c>
       <c r="C12" t="str">
-        <f>IF(ISBLANK(Library!B20),"",CONCATENATE("barcode",Library!E20))</f>
+        <f>IF(OR(ISBLANK(Library!E20),ISBLANK(Library!B20)),"",CONCATENATE("barcode",TEXT(Library!E20,"00")))</f>
         <v/>
       </c>
       <c r="D12" t="str">
@@ -2826,7 +3568,7 @@
         <v/>
       </c>
       <c r="C13" t="str">
-        <f>IF(ISBLANK(Library!B21),"",CONCATENATE("barcode",Library!E21))</f>
+        <f>IF(OR(ISBLANK(Library!E21),ISBLANK(Library!B21)),"",CONCATENATE("barcode",TEXT(Library!E21,"00")))</f>
         <v/>
       </c>
       <c r="D13" t="str">
@@ -2844,7 +3586,7 @@
         <v/>
       </c>
       <c r="C14" t="str">
-        <f>IF(ISBLANK(Library!B22),"",CONCATENATE("barcode",Library!E22))</f>
+        <f>IF(OR(ISBLANK(Library!E22),ISBLANK(Library!B22)),"",CONCATENATE("barcode",TEXT(Library!E22,"00")))</f>
         <v/>
       </c>
       <c r="D14" t="str">
@@ -2862,7 +3604,7 @@
         <v/>
       </c>
       <c r="C15" t="str">
-        <f>IF(ISBLANK(Library!B23),"",CONCATENATE("barcode",Library!E23))</f>
+        <f>IF(OR(ISBLANK(Library!E23),ISBLANK(Library!B23)),"",CONCATENATE("barcode",TEXT(Library!E23,"00")))</f>
         <v/>
       </c>
       <c r="D15" t="str">
@@ -2880,7 +3622,7 @@
         <v/>
       </c>
       <c r="C16" t="str">
-        <f>IF(ISBLANK(Library!B24),"",CONCATENATE("barcode",Library!E24))</f>
+        <f>IF(OR(ISBLANK(Library!E24),ISBLANK(Library!B24)),"",CONCATENATE("barcode",TEXT(Library!E24,"00")))</f>
         <v/>
       </c>
       <c r="D16" t="str">
@@ -2898,7 +3640,7 @@
         <v/>
       </c>
       <c r="C17" t="str">
-        <f>IF(ISBLANK(Library!B25),"",CONCATENATE("barcode",Library!E25))</f>
+        <f>IF(OR(ISBLANK(Library!E25),ISBLANK(Library!B25)),"",CONCATENATE("barcode",TEXT(Library!E25,"00")))</f>
         <v/>
       </c>
       <c r="D17" t="str">
@@ -2916,7 +3658,7 @@
         <v/>
       </c>
       <c r="C18" t="str">
-        <f>IF(ISBLANK(Library!B26),"",CONCATENATE("barcode",Library!E26))</f>
+        <f>IF(OR(ISBLANK(Library!E26),ISBLANK(Library!B26)),"",CONCATENATE("barcode",TEXT(Library!E26,"00")))</f>
         <v/>
       </c>
       <c r="D18" t="str">
@@ -2934,7 +3676,7 @@
         <v/>
       </c>
       <c r="C19" t="str">
-        <f>IF(ISBLANK(Library!B27),"",CONCATENATE("barcode",Library!E27))</f>
+        <f>IF(OR(ISBLANK(Library!E27),ISBLANK(Library!B27)),"",CONCATENATE("barcode",TEXT(Library!E27,"00")))</f>
         <v/>
       </c>
       <c r="D19" t="str">
@@ -2952,7 +3694,7 @@
         <v/>
       </c>
       <c r="C20" t="str">
-        <f>IF(ISBLANK(Library!B28),"",CONCATENATE("barcode",Library!E28))</f>
+        <f>IF(OR(ISBLANK(Library!E28),ISBLANK(Library!B28)),"",CONCATENATE("barcode",TEXT(Library!E28,"00")))</f>
         <v/>
       </c>
       <c r="D20" t="str">
@@ -2970,7 +3712,7 @@
         <v/>
       </c>
       <c r="C21" t="str">
-        <f>IF(ISBLANK(Library!B29),"",CONCATENATE("barcode",Library!E29))</f>
+        <f>IF(OR(ISBLANK(Library!E29),ISBLANK(Library!B29)),"",CONCATENATE("barcode",TEXT(Library!E29,"00")))</f>
         <v/>
       </c>
       <c r="D21" t="str">
@@ -2988,7 +3730,7 @@
         <v/>
       </c>
       <c r="C22" t="str">
-        <f>IF(ISBLANK(Library!B30),"",CONCATENATE("barcode",Library!E30))</f>
+        <f>IF(OR(ISBLANK(Library!E30),ISBLANK(Library!B30)),"",CONCATENATE("barcode",TEXT(Library!E30,"00")))</f>
         <v/>
       </c>
       <c r="D22" t="str">
@@ -3006,7 +3748,7 @@
         <v/>
       </c>
       <c r="C23" t="str">
-        <f>IF(ISBLANK(Library!B31),"",CONCATENATE("barcode",Library!E31))</f>
+        <f>IF(OR(ISBLANK(Library!E31),ISBLANK(Library!B31)),"",CONCATENATE("barcode",TEXT(Library!E31,"00")))</f>
         <v/>
       </c>
       <c r="D23" t="str">
@@ -3024,7 +3766,7 @@
         <v/>
       </c>
       <c r="C24" t="str">
-        <f>IF(ISBLANK(Library!B32),"",CONCATENATE("barcode",Library!E32))</f>
+        <f>IF(OR(ISBLANK(Library!E32),ISBLANK(Library!B32)),"",CONCATENATE("barcode",TEXT(Library!E32,"00")))</f>
         <v/>
       </c>
       <c r="D24" t="str">
@@ -3042,7 +3784,7 @@
         <v/>
       </c>
       <c r="C25" t="str">
-        <f>IF(ISBLANK(Library!B33),"",CONCATENATE("barcode",Library!E33))</f>
+        <f>IF(OR(ISBLANK(Library!E33),ISBLANK(Library!B33)),"",CONCATENATE("barcode",TEXT(Library!E33,"00")))</f>
         <v/>
       </c>
       <c r="D25" t="str">
@@ -3060,7 +3802,7 @@
         <v/>
       </c>
       <c r="C26" t="str">
-        <f>IF(ISBLANK(Library!B34),"",CONCATENATE("barcode",Library!E34))</f>
+        <f>IF(OR(ISBLANK(Library!E34),ISBLANK(Library!B34)),"",CONCATENATE("barcode",TEXT(Library!E34,"00")))</f>
         <v/>
       </c>
       <c r="D26" t="str">
@@ -3078,7 +3820,7 @@
         <v/>
       </c>
       <c r="C27" t="str">
-        <f>IF(ISBLANK(Library!B35),"",CONCATENATE("barcode",Library!E35))</f>
+        <f>IF(OR(ISBLANK(Library!E35),ISBLANK(Library!B35)),"",CONCATENATE("barcode",TEXT(Library!E35,"00")))</f>
         <v/>
       </c>
       <c r="D27" t="str">
@@ -3096,7 +3838,7 @@
         <v/>
       </c>
       <c r="C28" t="str">
-        <f>IF(ISBLANK(Library!B36),"",CONCATENATE("barcode",Library!E36))</f>
+        <f>IF(OR(ISBLANK(Library!E36),ISBLANK(Library!B36)),"",CONCATENATE("barcode",TEXT(Library!E36,"00")))</f>
         <v/>
       </c>
       <c r="D28" t="str">
@@ -3114,7 +3856,7 @@
         <v/>
       </c>
       <c r="C29" t="str">
-        <f>IF(ISBLANK(Library!B37),"",CONCATENATE("barcode",Library!E37))</f>
+        <f>IF(OR(ISBLANK(Library!E37),ISBLANK(Library!B37)),"",CONCATENATE("barcode",TEXT(Library!E37,"00")))</f>
         <v/>
       </c>
       <c r="D29" t="str">
@@ -3132,7 +3874,7 @@
         <v/>
       </c>
       <c r="C30" t="str">
-        <f>IF(ISBLANK(Library!B38),"",CONCATENATE("barcode",Library!E38))</f>
+        <f>IF(OR(ISBLANK(Library!E38),ISBLANK(Library!B38)),"",CONCATENATE("barcode",TEXT(Library!E38,"00")))</f>
         <v/>
       </c>
       <c r="D30" t="str">
@@ -3150,7 +3892,7 @@
         <v/>
       </c>
       <c r="C31" t="str">
-        <f>IF(ISBLANK(Library!B39),"",CONCATENATE("barcode",Library!E39))</f>
+        <f>IF(OR(ISBLANK(Library!E39),ISBLANK(Library!B39)),"",CONCATENATE("barcode",TEXT(Library!E39,"00")))</f>
         <v/>
       </c>
       <c r="D31" t="str">
@@ -3168,7 +3910,7 @@
         <v/>
       </c>
       <c r="C32" t="str">
-        <f>IF(ISBLANK(Library!B40),"",CONCATENATE("barcode",Library!E40))</f>
+        <f>IF(OR(ISBLANK(Library!E40),ISBLANK(Library!B40)),"",CONCATENATE("barcode",TEXT(Library!E40,"00")))</f>
         <v/>
       </c>
       <c r="D32" t="str">
@@ -3186,7 +3928,7 @@
         <v/>
       </c>
       <c r="C33" t="str">
-        <f>IF(ISBLANK(Library!B41),"",CONCATENATE("barcode",Library!E41))</f>
+        <f>IF(OR(ISBLANK(Library!E41),ISBLANK(Library!B41)),"",CONCATENATE("barcode",TEXT(Library!E41,"00")))</f>
         <v/>
       </c>
       <c r="D33" t="str">
@@ -3204,7 +3946,7 @@
         <v/>
       </c>
       <c r="C34" t="str">
-        <f>IF(ISBLANK(Library!B42),"",CONCATENATE("barcode",Library!E42))</f>
+        <f>IF(OR(ISBLANK(Library!E42),ISBLANK(Library!B42)),"",CONCATENATE("barcode",TEXT(Library!E42,"00")))</f>
         <v/>
       </c>
       <c r="D34" t="str">
@@ -3222,7 +3964,7 @@
         <v/>
       </c>
       <c r="C35" t="str">
-        <f>IF(ISBLANK(Library!B43),"",CONCATENATE("barcode",Library!E43))</f>
+        <f>IF(OR(ISBLANK(Library!E43),ISBLANK(Library!B43)),"",CONCATENATE("barcode",TEXT(Library!E43,"00")))</f>
         <v/>
       </c>
       <c r="D35" t="str">
@@ -3240,7 +3982,7 @@
         <v/>
       </c>
       <c r="C36" t="str">
-        <f>IF(ISBLANK(Library!B44),"",CONCATENATE("barcode",Library!E44))</f>
+        <f>IF(OR(ISBLANK(Library!E44),ISBLANK(Library!B44)),"",CONCATENATE("barcode",TEXT(Library!E44,"00")))</f>
         <v/>
       </c>
       <c r="D36" t="str">
@@ -3258,7 +4000,7 @@
         <v/>
       </c>
       <c r="C37" t="str">
-        <f>IF(ISBLANK(Library!B45),"",CONCATENATE("barcode",Library!E45))</f>
+        <f>IF(OR(ISBLANK(Library!E45),ISBLANK(Library!B45)),"",CONCATENATE("barcode",TEXT(Library!E45,"00")))</f>
         <v/>
       </c>
       <c r="D37" t="str">
@@ -3276,7 +4018,7 @@
         <v/>
       </c>
       <c r="C38" t="str">
-        <f>IF(ISBLANK(Library!B46),"",CONCATENATE("barcode",Library!E46))</f>
+        <f>IF(OR(ISBLANK(Library!E46),ISBLANK(Library!B46)),"",CONCATENATE("barcode",TEXT(Library!E46,"00")))</f>
         <v/>
       </c>
       <c r="D38" t="str">
@@ -3294,7 +4036,7 @@
         <v/>
       </c>
       <c r="C39" t="str">
-        <f>IF(ISBLANK(Library!B47),"",CONCATENATE("barcode",Library!E47))</f>
+        <f>IF(OR(ISBLANK(Library!E47),ISBLANK(Library!B47)),"",CONCATENATE("barcode",TEXT(Library!E47,"00")))</f>
         <v/>
       </c>
       <c r="D39" t="str">
@@ -3312,7 +4054,7 @@
         <v/>
       </c>
       <c r="C40" t="str">
-        <f>IF(ISBLANK(Library!B48),"",CONCATENATE("barcode",Library!E48))</f>
+        <f>IF(OR(ISBLANK(Library!E48),ISBLANK(Library!B48)),"",CONCATENATE("barcode",TEXT(Library!E48,"00")))</f>
         <v/>
       </c>
       <c r="D40" t="str">
@@ -3330,7 +4072,7 @@
         <v/>
       </c>
       <c r="C41" t="str">
-        <f>IF(ISBLANK(Library!B49),"",CONCATENATE("barcode",Library!E49))</f>
+        <f>IF(OR(ISBLANK(Library!E49),ISBLANK(Library!B49)),"",CONCATENATE("barcode",TEXT(Library!E49,"00")))</f>
         <v/>
       </c>
       <c r="D41" t="str">
@@ -3348,7 +4090,7 @@
         <v/>
       </c>
       <c r="C42" t="str">
-        <f>IF(ISBLANK(Library!B50),"",CONCATENATE("barcode",Library!E50))</f>
+        <f>IF(OR(ISBLANK(Library!E50),ISBLANK(Library!B50)),"",CONCATENATE("barcode",TEXT(Library!E50,"00")))</f>
         <v/>
       </c>
       <c r="D42" t="str">
@@ -3366,7 +4108,7 @@
         <v/>
       </c>
       <c r="C43" t="str">
-        <f>IF(ISBLANK(Library!B51),"",CONCATENATE("barcode",Library!E51))</f>
+        <f>IF(OR(ISBLANK(Library!E51),ISBLANK(Library!B51)),"",CONCATENATE("barcode",TEXT(Library!E51,"00")))</f>
         <v/>
       </c>
       <c r="D43" t="str">
@@ -3384,7 +4126,7 @@
         <v/>
       </c>
       <c r="C44" t="str">
-        <f>IF(ISBLANK(Library!B52),"",CONCATENATE("barcode",Library!E52))</f>
+        <f>IF(OR(ISBLANK(Library!E52),ISBLANK(Library!B52)),"",CONCATENATE("barcode",TEXT(Library!E52,"00")))</f>
         <v/>
       </c>
       <c r="D44" t="str">
@@ -3402,7 +4144,7 @@
         <v/>
       </c>
       <c r="C45" t="str">
-        <f>IF(ISBLANK(Library!B53),"",CONCATENATE("barcode",Library!E53))</f>
+        <f>IF(OR(ISBLANK(Library!E53),ISBLANK(Library!B53)),"",CONCATENATE("barcode",TEXT(Library!E53,"00")))</f>
         <v/>
       </c>
       <c r="D45" t="str">
@@ -3420,7 +4162,7 @@
         <v/>
       </c>
       <c r="C46" t="str">
-        <f>IF(ISBLANK(Library!B54),"",CONCATENATE("barcode",Library!E54))</f>
+        <f>IF(OR(ISBLANK(Library!E54),ISBLANK(Library!B54)),"",CONCATENATE("barcode",TEXT(Library!E54,"00")))</f>
         <v/>
       </c>
       <c r="D46" t="str">
@@ -3438,7 +4180,7 @@
         <v/>
       </c>
       <c r="C47" t="str">
-        <f>IF(ISBLANK(Library!B55),"",CONCATENATE("barcode",Library!E55))</f>
+        <f>IF(OR(ISBLANK(Library!E55),ISBLANK(Library!B55)),"",CONCATENATE("barcode",TEXT(Library!E55,"00")))</f>
         <v/>
       </c>
       <c r="D47" t="str">
@@ -3456,7 +4198,7 @@
         <v/>
       </c>
       <c r="C48" t="str">
-        <f>IF(ISBLANK(Library!B56),"",CONCATENATE("barcode",Library!E56))</f>
+        <f>IF(OR(ISBLANK(Library!E56),ISBLANK(Library!B56)),"",CONCATENATE("barcode",TEXT(Library!E56,"00")))</f>
         <v/>
       </c>
       <c r="D48" t="str">
@@ -3474,7 +4216,7 @@
         <v/>
       </c>
       <c r="C49" t="str">
-        <f>IF(ISBLANK(Library!B57),"",CONCATENATE("barcode",Library!E57))</f>
+        <f>IF(OR(ISBLANK(Library!E57),ISBLANK(Library!B57)),"",CONCATENATE("barcode",TEXT(Library!E57,"00")))</f>
         <v/>
       </c>
       <c r="D49" t="str">
@@ -3492,7 +4234,7 @@
         <v/>
       </c>
       <c r="C50" t="str">
-        <f>IF(ISBLANK(Library!B58),"",CONCATENATE("barcode",Library!E58))</f>
+        <f>IF(OR(ISBLANK(Library!E58),ISBLANK(Library!B58)),"",CONCATENATE("barcode",TEXT(Library!E58,"00")))</f>
         <v/>
       </c>
       <c r="D50" t="str">
@@ -3510,7 +4252,7 @@
         <v/>
       </c>
       <c r="C51" t="str">
-        <f>IF(ISBLANK(Library!B59),"",CONCATENATE("barcode",Library!E59))</f>
+        <f>IF(OR(ISBLANK(Library!E59),ISBLANK(Library!B59)),"",CONCATENATE("barcode",TEXT(Library!E59,"00")))</f>
         <v/>
       </c>
       <c r="D51" t="str">
@@ -3528,7 +4270,7 @@
         <v/>
       </c>
       <c r="C52" t="str">
-        <f>IF(ISBLANK(Library!B60),"",CONCATENATE("barcode",Library!E60))</f>
+        <f>IF(OR(ISBLANK(Library!E60),ISBLANK(Library!B60)),"",CONCATENATE("barcode",TEXT(Library!E60,"00")))</f>
         <v/>
       </c>
       <c r="D52" t="str">
@@ -3546,7 +4288,7 @@
         <v/>
       </c>
       <c r="C53" t="str">
-        <f>IF(ISBLANK(Library!B61),"",CONCATENATE("barcode",Library!E61))</f>
+        <f>IF(OR(ISBLANK(Library!E61),ISBLANK(Library!B61)),"",CONCATENATE("barcode",TEXT(Library!E61,"00")))</f>
         <v/>
       </c>
       <c r="D53" t="str">
@@ -3564,7 +4306,7 @@
         <v/>
       </c>
       <c r="C54" t="str">
-        <f>IF(ISBLANK(Library!B62),"",CONCATENATE("barcode",Library!E62))</f>
+        <f>IF(OR(ISBLANK(Library!E62),ISBLANK(Library!B62)),"",CONCATENATE("barcode",TEXT(Library!E62,"00")))</f>
         <v/>
       </c>
       <c r="D54" t="str">
@@ -3582,7 +4324,7 @@
         <v/>
       </c>
       <c r="C55" t="str">
-        <f>IF(ISBLANK(Library!B63),"",CONCATENATE("barcode",Library!E63))</f>
+        <f>IF(OR(ISBLANK(Library!E63),ISBLANK(Library!B63)),"",CONCATENATE("barcode",TEXT(Library!E63,"00")))</f>
         <v/>
       </c>
       <c r="D55" t="str">
@@ -3600,7 +4342,7 @@
         <v/>
       </c>
       <c r="C56" t="str">
-        <f>IF(ISBLANK(Library!B64),"",CONCATENATE("barcode",Library!E64))</f>
+        <f>IF(OR(ISBLANK(Library!E64),ISBLANK(Library!B64)),"",CONCATENATE("barcode",TEXT(Library!E64,"00")))</f>
         <v/>
       </c>
       <c r="D56" t="str">
@@ -3618,7 +4360,7 @@
         <v/>
       </c>
       <c r="C57" t="str">
-        <f>IF(ISBLANK(Library!B65),"",CONCATENATE("barcode",Library!E65))</f>
+        <f>IF(OR(ISBLANK(Library!E65),ISBLANK(Library!B65)),"",CONCATENATE("barcode",TEXT(Library!E65,"00")))</f>
         <v/>
       </c>
       <c r="D57" t="str">
@@ -3636,7 +4378,7 @@
         <v/>
       </c>
       <c r="C58" t="str">
-        <f>IF(ISBLANK(Library!B66),"",CONCATENATE("barcode",Library!E66))</f>
+        <f>IF(OR(ISBLANK(Library!E66),ISBLANK(Library!B66)),"",CONCATENATE("barcode",TEXT(Library!E66,"00")))</f>
         <v/>
       </c>
       <c r="D58" t="str">
@@ -3654,7 +4396,7 @@
         <v/>
       </c>
       <c r="C59" t="str">
-        <f>IF(ISBLANK(Library!B67),"",CONCATENATE("barcode",Library!E67))</f>
+        <f>IF(OR(ISBLANK(Library!E67),ISBLANK(Library!B67)),"",CONCATENATE("barcode",TEXT(Library!E67,"00")))</f>
         <v/>
       </c>
       <c r="D59" t="str">
@@ -3672,7 +4414,7 @@
         <v/>
       </c>
       <c r="C60" t="str">
-        <f>IF(ISBLANK(Library!B68),"",CONCATENATE("barcode",Library!E68))</f>
+        <f>IF(OR(ISBLANK(Library!E68),ISBLANK(Library!B68)),"",CONCATENATE("barcode",TEXT(Library!E68,"00")))</f>
         <v/>
       </c>
       <c r="D60" t="str">
@@ -3690,7 +4432,7 @@
         <v/>
       </c>
       <c r="C61" t="str">
-        <f>IF(ISBLANK(Library!B69),"",CONCATENATE("barcode",Library!E69))</f>
+        <f>IF(OR(ISBLANK(Library!E69),ISBLANK(Library!B69)),"",CONCATENATE("barcode",TEXT(Library!E69,"00")))</f>
         <v/>
       </c>
       <c r="D61" t="str">
@@ -3708,7 +4450,7 @@
         <v/>
       </c>
       <c r="C62" t="str">
-        <f>IF(ISBLANK(Library!B70),"",CONCATENATE("barcode",Library!E70))</f>
+        <f>IF(OR(ISBLANK(Library!E70),ISBLANK(Library!B70)),"",CONCATENATE("barcode",TEXT(Library!E70,"00")))</f>
         <v/>
       </c>
       <c r="D62" t="str">
@@ -3726,7 +4468,7 @@
         <v/>
       </c>
       <c r="C63" t="str">
-        <f>IF(ISBLANK(Library!B71),"",CONCATENATE("barcode",Library!E71))</f>
+        <f>IF(OR(ISBLANK(Library!E71),ISBLANK(Library!B71)),"",CONCATENATE("barcode",TEXT(Library!E71,"00")))</f>
         <v/>
       </c>
       <c r="D63" t="str">
@@ -3744,7 +4486,7 @@
         <v/>
       </c>
       <c r="C64" t="str">
-        <f>IF(ISBLANK(Library!B72),"",CONCATENATE("barcode",Library!E72))</f>
+        <f>IF(OR(ISBLANK(Library!E72),ISBLANK(Library!B72)),"",CONCATENATE("barcode",TEXT(Library!E72,"00")))</f>
         <v/>
       </c>
       <c r="D64" t="str">
@@ -3762,7 +4504,7 @@
         <v/>
       </c>
       <c r="C65" t="str">
-        <f>IF(ISBLANK(Library!B73),"",CONCATENATE("barcode",Library!E73))</f>
+        <f>IF(OR(ISBLANK(Library!E73),ISBLANK(Library!B73)),"",CONCATENATE("barcode",TEXT(Library!E73,"00")))</f>
         <v/>
       </c>
       <c r="D65" t="str">
@@ -3780,7 +4522,7 @@
         <v/>
       </c>
       <c r="C66" t="str">
-        <f>IF(ISBLANK(Library!B74),"",CONCATENATE("barcode",Library!E74))</f>
+        <f>IF(OR(ISBLANK(Library!E74),ISBLANK(Library!B74)),"",CONCATENATE("barcode",TEXT(Library!E74,"00")))</f>
         <v/>
       </c>
       <c r="D66" t="str">
@@ -3798,7 +4540,7 @@
         <v/>
       </c>
       <c r="C67" t="str">
-        <f>IF(ISBLANK(Library!B75),"",CONCATENATE("barcode",Library!E75))</f>
+        <f>IF(OR(ISBLANK(Library!E75),ISBLANK(Library!B75)),"",CONCATENATE("barcode",TEXT(Library!E75,"00")))</f>
         <v/>
       </c>
       <c r="D67" t="str">
@@ -3816,7 +4558,7 @@
         <v/>
       </c>
       <c r="C68" t="str">
-        <f>IF(ISBLANK(Library!B76),"",CONCATENATE("barcode",Library!E76))</f>
+        <f>IF(OR(ISBLANK(Library!E76),ISBLANK(Library!B76)),"",CONCATENATE("barcode",TEXT(Library!E76,"00")))</f>
         <v/>
       </c>
       <c r="D68" t="str">
@@ -3834,7 +4576,7 @@
         <v/>
       </c>
       <c r="C69" t="str">
-        <f>IF(ISBLANK(Library!B77),"",CONCATENATE("barcode",Library!E77))</f>
+        <f>IF(OR(ISBLANK(Library!E77),ISBLANK(Library!B77)),"",CONCATENATE("barcode",TEXT(Library!E77,"00")))</f>
         <v/>
       </c>
       <c r="D69" t="str">
@@ -3852,7 +4594,7 @@
         <v/>
       </c>
       <c r="C70" t="str">
-        <f>IF(ISBLANK(Library!B78),"",CONCATENATE("barcode",Library!E78))</f>
+        <f>IF(OR(ISBLANK(Library!E78),ISBLANK(Library!B78)),"",CONCATENATE("barcode",TEXT(Library!E78,"00")))</f>
         <v/>
       </c>
       <c r="D70" t="str">
@@ -3870,7 +4612,7 @@
         <v/>
       </c>
       <c r="C71" t="str">
-        <f>IF(ISBLANK(Library!B79),"",CONCATENATE("barcode",Library!E79))</f>
+        <f>IF(OR(ISBLANK(Library!E79),ISBLANK(Library!B79)),"",CONCATENATE("barcode",TEXT(Library!E79,"00")))</f>
         <v/>
       </c>
       <c r="D71" t="str">
@@ -3888,7 +4630,7 @@
         <v/>
       </c>
       <c r="C72" t="str">
-        <f>IF(ISBLANK(Library!B80),"",CONCATENATE("barcode",Library!E80))</f>
+        <f>IF(OR(ISBLANK(Library!E80),ISBLANK(Library!B80)),"",CONCATENATE("barcode",TEXT(Library!E80,"00")))</f>
         <v/>
       </c>
       <c r="D72" t="str">
@@ -3906,7 +4648,7 @@
         <v/>
       </c>
       <c r="C73" t="str">
-        <f>IF(ISBLANK(Library!B81),"",CONCATENATE("barcode",Library!E81))</f>
+        <f>IF(OR(ISBLANK(Library!E81),ISBLANK(Library!B81)),"",CONCATENATE("barcode",TEXT(Library!E81,"00")))</f>
         <v/>
       </c>
       <c r="D73" t="str">
@@ -3924,7 +4666,7 @@
         <v/>
       </c>
       <c r="C74" t="str">
-        <f>IF(ISBLANK(Library!B82),"",CONCATENATE("barcode",Library!E82))</f>
+        <f>IF(OR(ISBLANK(Library!E82),ISBLANK(Library!B82)),"",CONCATENATE("barcode",TEXT(Library!E82,"00")))</f>
         <v/>
       </c>
       <c r="D74" t="str">
@@ -3942,7 +4684,7 @@
         <v/>
       </c>
       <c r="C75" t="str">
-        <f>IF(ISBLANK(Library!B83),"",CONCATENATE("barcode",Library!E83))</f>
+        <f>IF(OR(ISBLANK(Library!E83),ISBLANK(Library!B83)),"",CONCATENATE("barcode",TEXT(Library!E83,"00")))</f>
         <v/>
       </c>
       <c r="D75" t="str">
@@ -3960,7 +4702,7 @@
         <v/>
       </c>
       <c r="C76" t="str">
-        <f>IF(ISBLANK(Library!B84),"",CONCATENATE("barcode",Library!E84))</f>
+        <f>IF(OR(ISBLANK(Library!E84),ISBLANK(Library!B84)),"",CONCATENATE("barcode",TEXT(Library!E84,"00")))</f>
         <v/>
       </c>
       <c r="D76" t="str">
@@ -3978,7 +4720,7 @@
         <v/>
       </c>
       <c r="C77" t="str">
-        <f>IF(ISBLANK(Library!B85),"",CONCATENATE("barcode",Library!E85))</f>
+        <f>IF(OR(ISBLANK(Library!E85),ISBLANK(Library!B85)),"",CONCATENATE("barcode",TEXT(Library!E85,"00")))</f>
         <v/>
       </c>
       <c r="D77" t="str">
@@ -3996,7 +4738,7 @@
         <v/>
       </c>
       <c r="C78" t="str">
-        <f>IF(ISBLANK(Library!B86),"",CONCATENATE("barcode",Library!E86))</f>
+        <f>IF(OR(ISBLANK(Library!E86),ISBLANK(Library!B86)),"",CONCATENATE("barcode",TEXT(Library!E86,"00")))</f>
         <v/>
       </c>
       <c r="D78" t="str">
@@ -4014,7 +4756,7 @@
         <v/>
       </c>
       <c r="C79" t="str">
-        <f>IF(ISBLANK(Library!B87),"",CONCATENATE("barcode",Library!E87))</f>
+        <f>IF(OR(ISBLANK(Library!E87),ISBLANK(Library!B87)),"",CONCATENATE("barcode",TEXT(Library!E87,"00")))</f>
         <v/>
       </c>
       <c r="D79" t="str">
@@ -4032,7 +4774,7 @@
         <v/>
       </c>
       <c r="C80" t="str">
-        <f>IF(ISBLANK(Library!B88),"",CONCATENATE("barcode",Library!E88))</f>
+        <f>IF(OR(ISBLANK(Library!E88),ISBLANK(Library!B88)),"",CONCATENATE("barcode",TEXT(Library!E88,"00")))</f>
         <v/>
       </c>
       <c r="D80" t="str">
@@ -4050,7 +4792,7 @@
         <v/>
       </c>
       <c r="C81" t="str">
-        <f>IF(ISBLANK(Library!B89),"",CONCATENATE("barcode",Library!E89))</f>
+        <f>IF(OR(ISBLANK(Library!E89),ISBLANK(Library!B89)),"",CONCATENATE("barcode",TEXT(Library!E89,"00")))</f>
         <v/>
       </c>
       <c r="D81" t="str">
@@ -4068,7 +4810,7 @@
         <v/>
       </c>
       <c r="C82" t="str">
-        <f>IF(ISBLANK(Library!B90),"",CONCATENATE("barcode",Library!E90))</f>
+        <f>IF(OR(ISBLANK(Library!E90),ISBLANK(Library!B90)),"",CONCATENATE("barcode",TEXT(Library!E90,"00")))</f>
         <v/>
       </c>
       <c r="D82" t="str">
@@ -4086,7 +4828,7 @@
         <v/>
       </c>
       <c r="C83" t="str">
-        <f>IF(ISBLANK(Library!B91),"",CONCATENATE("barcode",Library!E91))</f>
+        <f>IF(OR(ISBLANK(Library!E91),ISBLANK(Library!B91)),"",CONCATENATE("barcode",TEXT(Library!E91,"00")))</f>
         <v/>
       </c>
       <c r="D83" t="str">
@@ -4104,7 +4846,7 @@
         <v/>
       </c>
       <c r="C84" t="str">
-        <f>IF(ISBLANK(Library!B92),"",CONCATENATE("barcode",Library!E92))</f>
+        <f>IF(OR(ISBLANK(Library!E92),ISBLANK(Library!B92)),"",CONCATENATE("barcode",TEXT(Library!E92,"00")))</f>
         <v/>
       </c>
       <c r="D84" t="str">
@@ -4122,7 +4864,7 @@
         <v/>
       </c>
       <c r="C85" t="str">
-        <f>IF(ISBLANK(Library!B93),"",CONCATENATE("barcode",Library!E93))</f>
+        <f>IF(OR(ISBLANK(Library!E93),ISBLANK(Library!B93)),"",CONCATENATE("barcode",TEXT(Library!E93,"00")))</f>
         <v/>
       </c>
       <c r="D85" t="str">
@@ -4140,7 +4882,7 @@
         <v/>
       </c>
       <c r="C86" t="str">
-        <f>IF(ISBLANK(Library!B94),"",CONCATENATE("barcode",Library!E94))</f>
+        <f>IF(OR(ISBLANK(Library!E94),ISBLANK(Library!B94)),"",CONCATENATE("barcode",TEXT(Library!E94,"00")))</f>
         <v/>
       </c>
       <c r="D86" t="str">
@@ -4158,7 +4900,7 @@
         <v/>
       </c>
       <c r="C87" t="str">
-        <f>IF(ISBLANK(Library!B95),"",CONCATENATE("barcode",Library!E95))</f>
+        <f>IF(OR(ISBLANK(Library!E95),ISBLANK(Library!B95)),"",CONCATENATE("barcode",TEXT(Library!E95,"00")))</f>
         <v/>
       </c>
       <c r="D87" t="str">
@@ -4176,7 +4918,7 @@
         <v/>
       </c>
       <c r="C88" t="str">
-        <f>IF(ISBLANK(Library!B96),"",CONCATENATE("barcode",Library!E96))</f>
+        <f>IF(OR(ISBLANK(Library!E96),ISBLANK(Library!B96)),"",CONCATENATE("barcode",TEXT(Library!E96,"00")))</f>
         <v/>
       </c>
       <c r="D88" t="str">
@@ -4194,7 +4936,7 @@
         <v/>
       </c>
       <c r="C89" t="str">
-        <f>IF(ISBLANK(Library!B97),"",CONCATENATE("barcode",Library!E97))</f>
+        <f>IF(OR(ISBLANK(Library!E97),ISBLANK(Library!B97)),"",CONCATENATE("barcode",TEXT(Library!E97,"00")))</f>
         <v/>
       </c>
       <c r="D89" t="str">
@@ -4212,7 +4954,7 @@
         <v/>
       </c>
       <c r="C90" t="str">
-        <f>IF(ISBLANK(Library!B98),"",CONCATENATE("barcode",Library!E98))</f>
+        <f>IF(OR(ISBLANK(Library!E98),ISBLANK(Library!B98)),"",CONCATENATE("barcode",TEXT(Library!E98,"00")))</f>
         <v/>
       </c>
       <c r="D90" t="str">
@@ -4230,7 +4972,7 @@
         <v/>
       </c>
       <c r="C91" t="str">
-        <f>IF(ISBLANK(Library!B99),"",CONCATENATE("barcode",Library!E99))</f>
+        <f>IF(OR(ISBLANK(Library!E99),ISBLANK(Library!B99)),"",CONCATENATE("barcode",TEXT(Library!E99,"00")))</f>
         <v/>
       </c>
       <c r="D91" t="str">
@@ -4248,7 +4990,7 @@
         <v/>
       </c>
       <c r="C92" t="str">
-        <f>IF(ISBLANK(Library!B100),"",CONCATENATE("barcode",Library!E100))</f>
+        <f>IF(OR(ISBLANK(Library!E100),ISBLANK(Library!B100)),"",CONCATENATE("barcode",TEXT(Library!E100,"00")))</f>
         <v/>
       </c>
       <c r="D92" t="str">
@@ -4266,7 +5008,7 @@
         <v/>
       </c>
       <c r="C93" t="str">
-        <f>IF(ISBLANK(Library!B101),"",CONCATENATE("barcode",Library!E101))</f>
+        <f>IF(OR(ISBLANK(Library!E101),ISBLANK(Library!B101)),"",CONCATENATE("barcode",TEXT(Library!E101,"00")))</f>
         <v/>
       </c>
       <c r="D93" t="str">
@@ -4284,7 +5026,7 @@
         <v/>
       </c>
       <c r="C94" t="str">
-        <f>IF(ISBLANK(Library!B102),"",CONCATENATE("barcode",Library!E102))</f>
+        <f>IF(OR(ISBLANK(Library!E102),ISBLANK(Library!B102)),"",CONCATENATE("barcode",TEXT(Library!E102,"00")))</f>
         <v/>
       </c>
       <c r="D94" t="str">
@@ -4302,7 +5044,7 @@
         <v/>
       </c>
       <c r="C95" t="str">
-        <f>IF(ISBLANK(Library!B103),"",CONCATENATE("barcode",Library!E103))</f>
+        <f>IF(OR(ISBLANK(Library!E103),ISBLANK(Library!B103)),"",CONCATENATE("barcode",TEXT(Library!E103,"00")))</f>
         <v/>
       </c>
       <c r="D95" t="str">
@@ -4320,7 +5062,7 @@
         <v/>
       </c>
       <c r="C96" t="str">
-        <f>IF(ISBLANK(Library!B104),"",CONCATENATE("barcode",Library!E104))</f>
+        <f>IF(OR(ISBLANK(Library!E104),ISBLANK(Library!B104)),"",CONCATENATE("barcode",TEXT(Library!E104,"00")))</f>
         <v/>
       </c>
       <c r="D96" t="str">
@@ -4338,7 +5080,7 @@
         <v/>
       </c>
       <c r="C97" t="str">
-        <f>IF(ISBLANK(Library!B105),"",CONCATENATE("barcode",Library!E105))</f>
+        <f>IF(OR(ISBLANK(Library!E105),ISBLANK(Library!B105)),"",CONCATENATE("barcode",TEXT(Library!E105,"00")))</f>
         <v/>
       </c>
       <c r="D97" t="str">
@@ -4347,7 +5089,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3xPQ0b/tzn2kRstiisI5HHKRKYVCEvOGymGQwNY2weE/jCwbruWXpkygkZK3e21pFAqn9yoB182oDFvW5Xo9ow==" saltValue="VKYPjxAFkfQaTkoj0oFaAg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="BpfvFrrqtm0e7cxfocp+zTlVzBFfRuOvKl+EL7COePiHLmFrI52KWVpK8pzpUPY55InciSWy/Tz3uw4ktCZaQw==" saltValue="yEn5Lf0eHnWThP25T0izmg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
@@ -4381,7 +5123,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="22" t="s">
         <v>105</v>
       </c>
     </row>
@@ -4413,7 +5155,7 @@
   </sheetPr>
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -4423,50 +5165,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="25" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="26" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="26" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="36"/>
+      <c r="A4" s="27"/>
     </row>
     <row r="5" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="28" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="24" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="26" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="23" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="147" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="23" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="23" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4476,7 +5218,7 @@
       </c>
     </row>
     <row r="12" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="26" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed min sample_id length check
</commit_message>
<xml_diff>
--- a/src/nomadic/start/data/NOMADS_Library_Worksheet.xlsx
+++ b/src/nomadic/start/data/NOMADS_Library_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\nomadic\src\nomadic\start\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF95496-F69D-4D43-B9B0-81328E6CE62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE93DA-A7C3-4D03-B2EC-44744C34098F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46284" windowHeight="23244" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -943,12 +943,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
@@ -961,17 +972,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1758,25 +1758,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1785,34 +1785,34 @@
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
       <c r="E3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
       <c r="E4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="6" t="s">
         <v>129</v>
       </c>
@@ -1821,12 +1821,12 @@
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
       <c r="E6" s="5" t="s">
         <v>125</v>
       </c>
@@ -1835,15 +1835,15 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="43" t="str">
+      <c r="B7" s="43"/>
+      <c r="C7" s="46" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4), ISBLANK(C5), ISBLANK(C6)),"",CONCATENATE(C2,"_",C3,TEXT(C5,"000"),"_",C4,"_Batch",C6))</f>
         <v/>
       </c>
-      <c r="D7" s="43"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="5" t="s">
         <v>136</v>
       </c>
@@ -4586,8 +4586,13 @@
       <c r="I115" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A1:I1"/>
@@ -4595,12 +4600,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="B10:E105">
@@ -4631,9 +4630,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" error="The sample ID appears to be too short." prompt="Enter the Extraction ID" sqref="B10:B105" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>3</formula1>
-    </dataValidation>
+    <dataValidation errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showErrorMessage="1" error="The sample ID appears to be too short." prompt="Enter the Extraction ID" sqref="B10:B105" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Format" error="Exp Number should be three digits long" sqref="C6 E7:H7 I8" xr:uid="{7F700A24-FACB-40FF-A73D-3494166CE29A}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." sqref="C6 E7:H7 I8" xr:uid="{9C75F18E-0FA2-45C4-8859-DF7209A58F83}"/>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a Number" error="Please enter a number (decimal or whole) for the post-PCR DNA concentration" sqref="E10:E105" xr:uid="{10D485B7-FF0F-4E67-AF1B-44C96547CAC9}">

</xml_diff>